<commit_message>
evaluate with accuracy in classifier
</commit_message>
<xml_diff>
--- a/ADMET_bp.xlsx
+++ b/ADMET_bp.xlsx
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -616,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -874,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -893,10 +893,10 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -962,10 +962,10 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -981,13 +981,13 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1248,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -1270,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -1496,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1518,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">

</xml_diff>